<commit_message>
#00001-Updated main project as of 11-19-2020
</commit_message>
<xml_diff>
--- a/Document.xlsx
+++ b/Document.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\JP Files\Programs\TINPOS_Project\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="11460"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="Work logs" sheetId="3" r:id="rId1"/>
     <sheet name="Access Rights" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Accounting</t>
   </si>
@@ -175,14 +170,67 @@
   </si>
   <si>
     <t>Stopped in using c_Encryption to other forms.</t>
+  </si>
+  <si>
+    <t>In Connection string, Important: Open the TCP and UDP port of the SQL SERVER COMPUTER.</t>
+  </si>
+  <si>
+    <t>Created tables S01 to S03</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>Work done</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">c_Database.cs and c_TX_Database.cs </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Classes for Database functions</t>
+    </r>
+  </si>
+  <si>
+    <t>c_Shared - Functions that will be used all over the project</t>
+  </si>
+  <si>
+    <t>Screen CustomerRecord.cs has been created.</t>
+  </si>
+  <si>
+    <t>Created a function to Add S01.
+          Error occurred. StackOverflow</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -210,11 +258,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -275,7 +326,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -310,7 +361,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -487,7 +538,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -495,28 +546,85 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.85546875" style="3" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="2" max="2" width="45.85546875" style="4" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>53</v>
+      </c>
+    </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
         <v>43988</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
         <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
+        <v>44023</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>44023</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>44023</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>44054</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>44085</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>44085</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -524,7 +632,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>

</xml_diff>